<commit_message>
DML do bd/correções na modelagem
</commit_message>
<xml_diff>
--- a/bd/modelagem/modelagem_fisico.xlsx
+++ b/bd/modelagem/modelagem_fisico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Eduardo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Eduardo\Desktop\projeto_fcamara_squad42\bd\modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8353DBF-9B30-44AA-9C9B-AC2315B768F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B24B6-D0A2-406A-9A2E-45EDEB3C5ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{3880CC18-C042-494B-B891-FE3EAD04C1B6}"/>
+    <workbookView xWindow="23880" yWindow="1890" windowWidth="20730" windowHeight="11310" xr2:uid="{3880CC18-C042-494B-B891-FE3EAD04C1B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Santos</t>
   </si>
   <si>
-    <t>EndereçoEscritorio</t>
-  </si>
-  <si>
     <t>R. Bela Cintra, 986 - 2° andar</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Tarde</t>
+  </si>
+  <si>
+    <t>EnderecoEscritorio</t>
   </si>
 </sst>
 </file>
@@ -314,9 +314,6 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,9 +321,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,9 +328,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,9 +343,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,9 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,6 +362,24 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -710,7 +710,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,323 +727,323 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="D1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="23"/>
+      <c r="G1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="D6" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="15">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="13">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="E10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="15">
         <v>4</v>
       </c>
-      <c r="D4" s="7">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="13">
-        <v>2</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="E11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="D6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>1</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="20">
-        <v>1</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>2</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="20">
-        <v>2</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="20">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="20">
+        <v>1</v>
+      </c>
+      <c r="E15" s="21">
+        <v>44449</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20">
+        <v>1</v>
+      </c>
+      <c r="H15" s="20">
+        <v>1</v>
+      </c>
+      <c r="I15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="20">
+        <v>2</v>
+      </c>
+      <c r="E16" s="21">
+        <v>44452</v>
+      </c>
+      <c r="F16" s="20">
+        <v>4</v>
+      </c>
+      <c r="G16" s="20">
+        <v>2</v>
+      </c>
+      <c r="H16" s="20">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="20">
         <v>3</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="20">
+      <c r="E17" s="21">
+        <v>44479</v>
+      </c>
+      <c r="F17" s="20">
+        <v>2</v>
+      </c>
+      <c r="G17" s="20">
+        <v>1</v>
+      </c>
+      <c r="H17" s="20">
+        <v>2</v>
+      </c>
+      <c r="I17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="20">
         <v>4</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="26">
-        <v>1</v>
-      </c>
-      <c r="E15" s="27">
-        <v>44449</v>
-      </c>
-      <c r="F15" s="26">
-        <v>1</v>
-      </c>
-      <c r="G15" s="26">
-        <v>1</v>
-      </c>
-      <c r="H15" s="26">
-        <v>1</v>
-      </c>
-      <c r="I15" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="26">
-        <v>2</v>
-      </c>
-      <c r="E16" s="27">
-        <v>44452</v>
-      </c>
-      <c r="F16" s="26">
-        <v>4</v>
-      </c>
-      <c r="G16" s="26">
-        <v>2</v>
-      </c>
-      <c r="H16" s="26">
-        <v>1</v>
-      </c>
-      <c r="I16" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="26">
-        <v>3</v>
-      </c>
-      <c r="E17" s="27">
-        <v>44479</v>
-      </c>
-      <c r="F17" s="26">
-        <v>2</v>
-      </c>
-      <c r="G17" s="26">
-        <v>1</v>
-      </c>
-      <c r="H17" s="26">
-        <v>2</v>
-      </c>
-      <c r="I17" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="26">
-        <v>4</v>
-      </c>
-      <c r="E18" s="27">
+      <c r="E18" s="21">
         <v>44478</v>
       </c>
-      <c r="F18" s="26">
-        <v>1</v>
-      </c>
-      <c r="G18" s="26">
-        <v>2</v>
-      </c>
-      <c r="H18" s="26">
-        <v>1</v>
-      </c>
-      <c r="I18" s="26">
+      <c r="F18" s="20">
+        <v>1</v>
+      </c>
+      <c r="G18" s="20">
+        <v>2</v>
+      </c>
+      <c r="H18" s="20">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D13:I13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D13:I13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{79D329C7-1397-4E47-9BF0-18DF5AD09C89}"/>

</xml_diff>